<commit_message>
-added a check for diversity between rounds -100% done!!!!!
</commit_message>
<xml_diff>
--- a/Delphi/data.xlsx
+++ b/Delphi/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hristos Birbou\PycharmProjects\legendary-rotary-phone\Delphi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7718FC00-FC22-46A8-B503-751848215D49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082E057D-C5A2-4DAC-8EAB-A450D76BFE7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33270" yWindow="3960" windowWidth="14895" windowHeight="8670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -387,7 +387,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D7"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,19 +420,19 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G2">
         <v>3</v>
@@ -446,16 +446,16 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -469,16 +469,16 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -501,10 +501,10 @@
         <v>2</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -521,7 +521,7 @@
         <v>4</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -535,19 +535,19 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <v>2</v>

</xml_diff>